<commit_message>
split VI and modified excels
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2542-MS-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DELETE-VAR-INST-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2542-MS-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DELETE-VAR-INST-Newcreateloan1.xlsx
@@ -200,14 +200,14 @@
     <t>deleterepaymentschedule</t>
   </si>
   <si>
-    <t>2460-RBI-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DATE-VAR-INST</t>
+    <t>2540-MS-EPP-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DATE-VAR-INST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +224,12 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -332,11 +338,13 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +670,7 @@
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>60</v>
       </c>
     </row>
@@ -710,7 +718,7 @@
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>10000</v>
       </c>
     </row>
@@ -1577,50 +1585,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1641,7 +1649,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1665,10 +1673,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>